<commit_message>
remove unused python library
</commit_message>
<xml_diff>
--- a/iNatStruct.xlsx
+++ b/iNatStruct.xlsx
@@ -199,64 +199,64 @@
     <t xml:space="preserve">             74.655070</t>
   </si>
   <si>
-    <t>[0.31, 0.35, 0.34]</t>
-  </si>
-  <si>
-    <t>[0.37, 0.4, 0.23]</t>
-  </si>
-  <si>
-    <t>[0.34, 0.35, 0.31]</t>
-  </si>
-  <si>
-    <t>[0.18, 0.6, 0.22]</t>
+    <t>[0.34, 0.31, 0.35]</t>
+  </si>
+  <si>
+    <t>[0.4, 0.37, 0.23]</t>
+  </si>
+  <si>
+    <t>[0.34, 0.32, 0.34]</t>
+  </si>
+  <si>
+    <t>[0.6, 0.18, 0.22]</t>
   </si>
   <si>
     <t>[0.63, 0.22, 0.14]</t>
   </si>
   <si>
-    <t>[0.38, 0.41, 0.2]</t>
-  </si>
-  <si>
-    <t>[0.15, 0.68, 0.17]</t>
+    <t>[0.38, 0.21, 0.41]</t>
+  </si>
+  <si>
+    <t>[0.68, 0.15, 0.17]</t>
   </si>
   <si>
     <t>[0.22, 0.6, 0.18]</t>
   </si>
   <si>
-    <t>[0.55, 0.1, 0.34]</t>
-  </si>
-  <si>
-    <t>[0.43, 0.45, 0.12]</t>
-  </si>
-  <si>
-    <t>['#3d4027', '#b8beb4', '#7e876e']</t>
-  </si>
-  <si>
-    <t>['#35411d', '#758251', '#bfc88a']</t>
-  </si>
-  <si>
-    <t>['#807660', '#c4bb9b', '#3d3a2b']</t>
-  </si>
-  <si>
-    <t>['#314d12', '#bfcede', '#628138']</t>
+    <t>[0.56, 0.1, 0.34]</t>
+  </si>
+  <si>
+    <t>[0.44, 0.45, 0.11]</t>
+  </si>
+  <si>
+    <t>['#7f886e', '#3d4127', '#b8beb4']</t>
+  </si>
+  <si>
+    <t>['#758251', '#35411d', '#bfc889']</t>
+  </si>
+  <si>
+    <t>['#c4bb9c', '#3e3b2d', '#827862']</t>
+  </si>
+  <si>
+    <t>['#bfcede', '#314d12', '#628138']</t>
   </si>
   <si>
     <t>['#bccadc', '#2a4913', '#a2b1bc']</t>
   </si>
   <si>
-    <t>['#ccc8c1', '#66784e', '#273714']</t>
-  </si>
-  <si>
-    <t>['#5d6c45', '#b8c7dc', '#373217']</t>
+    <t>['#ccc8c1', '#283714', '#66784e']</t>
+  </si>
+  <si>
+    <t>['#b8c7dc', '#5c6c44', '#373217']</t>
   </si>
   <si>
     <t>['#192718', '#adbbd2', '#99a7bc']</t>
   </si>
   <si>
-    <t>['#acbad2', '#3f3e2a', '#97a4ba']</t>
-  </si>
-  <si>
-    <t>['#bab9b6', '#8f8f8a', '#704f43']</t>
+    <t>['#acbad2', '#3f3e2a', '#97a4b9']</t>
+  </si>
+  <si>
+    <t>['#b9b8b5', '#8e8e88', '#704c3f']</t>
   </si>
 </sst>
 </file>
@@ -730,31 +730,31 @@
         <v>-76.4110874383</v>
       </c>
       <c r="J2">
-        <v>61.29928786254877</v>
+        <v>126.5631645844316</v>
       </c>
       <c r="K2">
-        <v>64.49839250526024</v>
+        <v>135.7539758812044</v>
       </c>
       <c r="L2">
-        <v>39.20468766203901</v>
+        <v>110.2767151315988</v>
       </c>
       <c r="M2">
-        <v>183.5505897913028</v>
+        <v>61.49758395955317</v>
       </c>
       <c r="N2">
-        <v>189.5492364240238</v>
+        <v>64.65939848329957</v>
       </c>
       <c r="O2">
-        <v>179.932516186573</v>
+        <v>39.38283493542211</v>
       </c>
       <c r="P2">
-        <v>126.3510205344849</v>
+        <v>183.6292628753858</v>
       </c>
       <c r="Q2">
-        <v>135.4956749145045</v>
+        <v>189.6336279363796</v>
       </c>
       <c r="R2">
-        <v>110.0047661049466</v>
+        <v>180.0335631545592</v>
       </c>
       <c r="S2" t="s">
         <v>61</v>
@@ -801,31 +801,31 @@
         <v>-76.411111596</v>
       </c>
       <c r="J3">
-        <v>53.24552056030928</v>
+        <v>116.8762323920106</v>
       </c>
       <c r="K3">
-        <v>64.83173634683813</v>
+        <v>130.04179096491</v>
       </c>
       <c r="L3">
-        <v>28.93991606869724</v>
+        <v>80.58489960269071</v>
       </c>
       <c r="M3">
-        <v>116.9171906354511</v>
+        <v>53.22184001949568</v>
       </c>
       <c r="N3">
-        <v>130.085846153845</v>
+        <v>64.81027934241865</v>
       </c>
       <c r="O3">
-        <v>80.61851505016641</v>
+        <v>28.92279027103484</v>
       </c>
       <c r="P3">
-        <v>191.2214017842582</v>
+        <v>191.1821714445269</v>
       </c>
       <c r="Q3">
-        <v>200.2590901679424</v>
+        <v>200.2241948994773</v>
       </c>
       <c r="R3">
-        <v>137.5250285341619</v>
+        <v>137.4939966492951</v>
       </c>
       <c r="S3" t="s">
         <v>62</v>
@@ -875,31 +875,31 @@
         <v>-76.4111424915</v>
       </c>
       <c r="J4">
-        <v>127.5648706998446</v>
+        <v>196.1845401388855</v>
       </c>
       <c r="K4">
-        <v>117.5441952818446</v>
+        <v>187.4492326503656</v>
       </c>
       <c r="L4">
-        <v>96.44549852656083</v>
+        <v>155.6496841247063</v>
       </c>
       <c r="M4">
-        <v>195.5144995036975</v>
+        <v>61.90421877825159</v>
       </c>
       <c r="N4">
-        <v>186.6339925173621</v>
+        <v>59.49599815932039</v>
       </c>
       <c r="O4">
-        <v>154.552905245463</v>
+        <v>44.64111624238532</v>
       </c>
       <c r="P4">
-        <v>60.72140441955506</v>
+        <v>130.0051064235949</v>
       </c>
       <c r="Q4">
-        <v>58.34024386079069</v>
+        <v>119.6158251407843</v>
       </c>
       <c r="R4">
-        <v>43.49748966836983</v>
+        <v>97.71941713594822</v>
       </c>
       <c r="S4" t="s">
         <v>63</v>
@@ -946,22 +946,22 @@
         <v>-80.40928359660001</v>
       </c>
       <c r="J5">
+        <v>191.3518264311085</v>
+      </c>
+      <c r="K5">
+        <v>206.0431961207371</v>
+      </c>
+      <c r="L5">
+        <v>221.9472304922189</v>
+      </c>
+      <c r="M5">
         <v>48.64646084337149</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>76.94636237256844</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>17.71605653384222</v>
-      </c>
-      <c r="M5">
-        <v>191.3518264311085</v>
-      </c>
-      <c r="N5">
-        <v>206.0431961207371</v>
-      </c>
-      <c r="O5">
-        <v>221.9472304922189</v>
       </c>
       <c r="P5">
         <v>97.96231550041296</v>
@@ -970,7 +970,7 @@
         <v>128.9413769430669</v>
       </c>
       <c r="R5">
-        <v>56.08100818909595</v>
+        <v>56.08100818909594</v>
       </c>
       <c r="S5" t="s">
         <v>64</v>
@@ -1026,22 +1026,22 @@
         <v>220.0308160196237</v>
       </c>
       <c r="M6">
-        <v>41.70671806954982</v>
+        <v>41.70808148114206</v>
       </c>
       <c r="N6">
-        <v>72.91763641989479</v>
+        <v>72.91859026225309</v>
       </c>
       <c r="O6">
-        <v>19.4729777967988</v>
+        <v>19.47520346483464</v>
       </c>
       <c r="P6">
-        <v>162.1790548204148</v>
+        <v>162.1814435328357</v>
       </c>
       <c r="Q6">
-        <v>176.7631758034032</v>
+        <v>176.7655866006281</v>
       </c>
       <c r="R6">
-        <v>187.6906238185244</v>
+        <v>187.6934477674003</v>
       </c>
       <c r="S6" t="s">
         <v>65</v>
@@ -1088,31 +1088,31 @@
         <v>-80.40952306609999</v>
       </c>
       <c r="J7">
-        <v>204.405057285193</v>
+        <v>204.4227235919868</v>
       </c>
       <c r="K7">
-        <v>200.2555715262557</v>
+        <v>200.2727221958501</v>
       </c>
       <c r="L7">
-        <v>192.8300004186434</v>
+        <v>192.8627732946076</v>
       </c>
       <c r="M7">
-        <v>101.7244597186253</v>
+        <v>39.58090791179841</v>
       </c>
       <c r="N7">
-        <v>119.6308452716525</v>
+        <v>54.97963683527826</v>
       </c>
       <c r="O7">
-        <v>77.74923736340824</v>
+        <v>20.33447470817669</v>
       </c>
       <c r="P7">
-        <v>39.25806028833108</v>
+        <v>101.9141017019259</v>
       </c>
       <c r="Q7">
-        <v>54.62374836172941</v>
+        <v>119.8082225440996</v>
       </c>
       <c r="R7">
-        <v>20.05030144168325</v>
+        <v>77.92479695826066</v>
       </c>
       <c r="S7" t="s">
         <v>66</v>
@@ -1162,31 +1162,31 @@
         <v>-80.4847910049</v>
       </c>
       <c r="J8">
-        <v>92.81340810603754</v>
+        <v>183.9214150159144</v>
       </c>
       <c r="K8">
-        <v>108.1964968500805</v>
+        <v>199.0223889960659</v>
       </c>
       <c r="L8">
-        <v>69.09562652490003</v>
+        <v>219.7645508869342</v>
       </c>
       <c r="M8">
-        <v>183.9482451528821</v>
+        <v>92.38540466589484</v>
       </c>
       <c r="N8">
-        <v>199.0503895737077</v>
+        <v>107.7785858294953</v>
       </c>
       <c r="O8">
-        <v>219.8042480403625</v>
+        <v>68.48819124424988</v>
       </c>
       <c r="P8">
-        <v>54.77215267549849</v>
+        <v>54.59066633546077</v>
       </c>
       <c r="Q8">
-        <v>50.0282891507143</v>
+        <v>49.60212382786062</v>
       </c>
       <c r="R8">
-        <v>22.77887211585968</v>
+        <v>22.57256411849005</v>
       </c>
       <c r="S8" t="s">
         <v>67</v>
@@ -1236,10 +1236,10 @@
         <v>24.62294724073291</v>
       </c>
       <c r="K9">
-        <v>39.45588841721809</v>
+        <v>39.45588841721808</v>
       </c>
       <c r="L9">
-        <v>24.08240145545858</v>
+        <v>24.08240145545861</v>
       </c>
       <c r="M9">
         <v>172.6558463915306</v>
@@ -1304,31 +1304,31 @@
         <v>-80.4095616039</v>
       </c>
       <c r="J10">
-        <v>171.6524343774405</v>
+        <v>171.5424700663058</v>
       </c>
       <c r="K10">
-        <v>186.0459767897252</v>
+        <v>185.9211849449001</v>
       </c>
       <c r="L10">
-        <v>209.8695459237344</v>
+        <v>209.7348184897223</v>
       </c>
       <c r="M10">
-        <v>62.50738639268459</v>
+        <v>62.50506083223027</v>
       </c>
       <c r="N10">
-        <v>61.79379440779776</v>
+        <v>61.79112565176095</v>
       </c>
       <c r="O10">
-        <v>41.63170270407647</v>
+        <v>41.62810551067622</v>
       </c>
       <c r="P10">
-        <v>151.0872798556223</v>
+        <v>150.8932243397807</v>
       </c>
       <c r="Q10">
-        <v>163.9499035409798</v>
+        <v>163.7523723523916</v>
       </c>
       <c r="R10">
-        <v>185.6025110461135</v>
+        <v>185.3814140646039</v>
       </c>
       <c r="S10" t="s">
         <v>69</v>
@@ -1375,31 +1375,31 @@
         <v>60</v>
       </c>
       <c r="J11">
-        <v>185.5686494715423</v>
+        <v>184.8598147768016</v>
       </c>
       <c r="K11">
-        <v>184.8934601130462</v>
+        <v>184.1953174996002</v>
       </c>
       <c r="L11">
-        <v>182.0654862176983</v>
+        <v>181.3286926912922</v>
       </c>
       <c r="M11">
-        <v>143.085148538344</v>
+        <v>141.6376205941343</v>
       </c>
       <c r="N11">
-        <v>142.9610383447226</v>
+        <v>141.5192234215295</v>
       </c>
       <c r="O11">
-        <v>137.9667449696287</v>
+        <v>136.4505802846509</v>
       </c>
       <c r="P11">
-        <v>112.4255190048968</v>
+        <v>112.4421615939599</v>
       </c>
       <c r="Q11">
-        <v>79.48836302170766</v>
+        <v>76.14897988436529</v>
       </c>
       <c r="R11">
-        <v>66.93546569584019</v>
+        <v>62.99483969612039</v>
       </c>
       <c r="S11" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Reorder columns and add place feature
</commit_message>
<xml_diff>
--- a/iNatStruct.xlsx
+++ b/iNatStruct.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="107">
   <si>
     <t>Image_Label</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Seconds</t>
   </si>
   <si>
-    <t>Annotations</t>
+    <t>Place</t>
   </si>
   <si>
     <t>Lat</t>
@@ -46,6 +46,9 @@
     <t>Long</t>
   </si>
   <si>
+    <t>Hex_Color_Code</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -91,18 +94,15 @@
     <t>Prop3</t>
   </si>
   <si>
-    <t>Hex_Color_Code</t>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
   <si>
     <t>Contour_Area</t>
   </si>
   <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
     <t>Aspect_Ratio</t>
   </si>
   <si>
@@ -247,85 +247,94 @@
     <t>10:23:00</t>
   </si>
   <si>
-    <t>[]</t>
+    <t>Highview Dr, Blacksburg, VA, US</t>
+  </si>
+  <si>
+    <t>Virginia, US</t>
   </si>
   <si>
     <t>Princeton University</t>
   </si>
   <si>
+    <t>Jefferson National Forest, Virginia 24134, USA</t>
+  </si>
+  <si>
+    <t>Giles County, VA, USA</t>
+  </si>
+  <si>
     <t xml:space="preserve">             40.343137</t>
   </si>
   <si>
     <t xml:space="preserve">             74.655070</t>
   </si>
   <si>
+    <t>['#bccbdd', '#2a4b13', '#a3b2bd']</t>
+  </si>
+  <si>
+    <t>['#b7c6db', '#393117', '#5c6c44']</t>
+  </si>
+  <si>
+    <t>['#9aa8bd', '#233827', '#adbcd2']</t>
+  </si>
+  <si>
+    <t>['#acbad2', '#3f3e2a', '#97a4ba']</t>
+  </si>
+  <si>
+    <t>['#7b859c', '#354723', '#9aa6c5']</t>
+  </si>
+  <si>
+    <t>['#828fa9', '#384935', '#8e9bbc']</t>
+  </si>
+  <si>
+    <t>['#dedad6', '#365b10', '#547528']</t>
+  </si>
+  <si>
+    <t>['#dbdad9', '#244a0f', '#859578']</t>
+  </si>
+  <si>
+    <t>['#d3d1ce', '#1b4009', '#4d6a28']</t>
+  </si>
+  <si>
+    <t>['#d7d2cd', '#54643a', '#3b4c1b']</t>
+  </si>
+  <si>
+    <t>['#b7b6b5', '#3d4924', '#c9c8c5']</t>
+  </si>
+  <si>
+    <t>['#294414', '#d1d0d0', '#a0a49d']</t>
+  </si>
+  <si>
+    <t>['#d1cdc8', '#22410c', '#7f8b77']</t>
+  </si>
+  <si>
+    <t>lightsteelblue</t>
+  </si>
+  <si>
     <t>darkgray</t>
   </si>
   <si>
-    <t>lightsteelblue</t>
+    <t>lightslategray</t>
+  </si>
+  <si>
+    <t>gainsboro</t>
+  </si>
+  <si>
+    <t>lightgray</t>
+  </si>
+  <si>
+    <t>silver</t>
+  </si>
+  <si>
+    <t>darkgreen</t>
+  </si>
+  <si>
+    <t>darkslategray</t>
   </si>
   <si>
     <t>darkolivegreen</t>
   </si>
   <si>
-    <t>darkgreen</t>
-  </si>
-  <si>
-    <t>lightgray</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
-    <t>darkslategray</t>
-  </si>
-  <si>
-    <t>lightslategray</t>
-  </si>
-  <si>
-    <t>gainsboro</t>
-  </si>
-  <si>
     <t>gray</t>
-  </si>
-  <si>
-    <t>['#a3b2bd', '#2a4b13', '#bccbdd']</t>
-  </si>
-  <si>
-    <t>['#b7c6db', '#5c6c44', '#393117']</t>
-  </si>
-  <si>
-    <t>['#adbcd2', '#233827', '#9aa8bd']</t>
-  </si>
-  <si>
-    <t>['#acbad2', '#3f3e2a', '#97a4ba']</t>
-  </si>
-  <si>
-    <t>['#9aa6c5', '#7b859c', '#354723']</t>
-  </si>
-  <si>
-    <t>['#8e9bbc', '#384935', '#828fa9']</t>
-  </si>
-  <si>
-    <t>['#365b10', '#dedad6', '#547528']</t>
-  </si>
-  <si>
-    <t>['#244a0f', '#dbdad9', '#859578']</t>
-  </si>
-  <si>
-    <t>['#d3d1ce', '#1b4009', '#4d6a28']</t>
-  </si>
-  <si>
-    <t>['#d7d2cd', '#546439', '#3b4c1b']</t>
-  </si>
-  <si>
-    <t>['#b7b6b5', '#c9c8c5', '#3d4924']</t>
-  </si>
-  <si>
-    <t>['#d1d0d0', '#294414', '#a0a49d']</t>
-  </si>
-  <si>
-    <t>['#d1cdc8', '#22410c', '#7f8c78']</t>
   </si>
 </sst>
 </file>
@@ -828,62 +837,62 @@
       <c r="J2">
         <v>-80.40952306609999</v>
       </c>
-      <c r="K2">
-        <v>188.3437748759284</v>
+      <c r="K2" t="s">
+        <v>84</v>
       </c>
       <c r="L2">
-        <v>202.8482461934476</v>
+        <v>188.3417578974903</v>
       </c>
       <c r="M2">
-        <v>220.9193130430371</v>
-      </c>
-      <c r="N2" t="s">
-        <v>81</v>
-      </c>
-      <c r="O2">
+        <v>202.8464697265992</v>
+      </c>
+      <c r="N2">
+        <v>220.9160168321952</v>
+      </c>
+      <c r="O2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2">
         <v>0.6489010989010989</v>
       </c>
-      <c r="P2">
-        <v>42.30053129512963</v>
-      </c>
       <c r="Q2">
-        <v>75.41380435288065</v>
+        <v>42.29902360588152</v>
       </c>
       <c r="R2">
-        <v>19.39029221232124</v>
-      </c>
-      <c r="S2" t="s">
-        <v>84</v>
-      </c>
-      <c r="T2">
+        <v>75.41250902988652</v>
+      </c>
+      <c r="S2">
+        <v>19.38843707034124</v>
+      </c>
+      <c r="T2" t="s">
+        <v>103</v>
+      </c>
+      <c r="U2">
         <v>0.2357857142857143</v>
       </c>
-      <c r="U2">
-        <v>163.2940952380957</v>
-      </c>
       <c r="V2">
-        <v>178.0078095238095</v>
+        <v>163.2776930409918</v>
       </c>
       <c r="W2">
-        <v>189.2647619047611</v>
-      </c>
-      <c r="X2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y2">
+        <v>177.9907054337464</v>
+      </c>
+      <c r="X2">
+        <v>189.2473307912289</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z2">
         <v>0.1153131868131868</v>
       </c>
-      <c r="Z2" t="s">
-        <v>91</v>
-      </c>
       <c r="AA2">
+        <v>272</v>
+      </c>
+      <c r="AB2">
+        <v>267</v>
+      </c>
+      <c r="AC2">
         <v>42647</v>
-      </c>
-      <c r="AB2">
-        <v>272</v>
-      </c>
-      <c r="AC2">
-        <v>267</v>
       </c>
       <c r="AD2">
         <v>1.0187265917603</v>
@@ -918,7 +927,7 @@
         <v>43743</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I3">
         <v>37.3504969752</v>
@@ -926,62 +935,62 @@
       <c r="J3">
         <v>-80.4847910049</v>
       </c>
-      <c r="K3">
-        <v>183.2364997904586</v>
+      <c r="K3" t="s">
+        <v>85</v>
       </c>
       <c r="L3">
-        <v>198.2781410869785</v>
+        <v>183.2323597318077</v>
       </c>
       <c r="M3">
-        <v>218.8874672824065</v>
-      </c>
-      <c r="N3" t="s">
-        <v>82</v>
-      </c>
-      <c r="O3">
-        <v>0.6690899470899471</v>
+        <v>198.2738788032164</v>
+      </c>
+      <c r="N3">
+        <v>218.8811673730186</v>
+      </c>
+      <c r="O3" t="s">
+        <v>97</v>
       </c>
       <c r="P3">
-        <v>57.41178645144289</v>
+        <v>0.6690952380952381</v>
       </c>
       <c r="Q3">
-        <v>48.628538862022</v>
+        <v>57.37200037061943</v>
       </c>
       <c r="R3">
-        <v>22.80003696743927</v>
-      </c>
-      <c r="S3" t="s">
-        <v>83</v>
-      </c>
-      <c r="T3">
-        <v>0.1723597883597884</v>
+        <v>48.5369529633434</v>
+      </c>
+      <c r="S3">
+        <v>22.76376663887243</v>
+      </c>
+      <c r="T3" t="s">
+        <v>104</v>
       </c>
       <c r="U3">
-        <v>92.19768601636036</v>
+        <v>0.171994708994709</v>
       </c>
       <c r="V3">
-        <v>107.803776846867</v>
+        <v>92.12995455902642</v>
       </c>
       <c r="W3">
-        <v>67.63780836492623</v>
-      </c>
-      <c r="X3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y3">
-        <v>0.1585502645502646</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>92</v>
+        <v>107.7260605658584</v>
+      </c>
+      <c r="X3">
+        <v>67.52605393214542</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z3">
+        <v>0.1589100529100529</v>
       </c>
       <c r="AA3">
+        <v>428</v>
+      </c>
+      <c r="AB3">
+        <v>465</v>
+      </c>
+      <c r="AC3">
         <v>60445</v>
-      </c>
-      <c r="AB3">
-        <v>428</v>
-      </c>
-      <c r="AC3">
-        <v>465</v>
       </c>
       <c r="AD3">
         <v>0.9204301075268817</v>
@@ -1021,62 +1030,62 @@
       <c r="J4">
         <v>-80.4092512154</v>
       </c>
-      <c r="K4">
-        <v>172.7767881710603</v>
+      <c r="K4" t="s">
+        <v>86</v>
       </c>
       <c r="L4">
-        <v>187.6401065878875</v>
+        <v>172.773271762652</v>
       </c>
       <c r="M4">
-        <v>210.2568825940269</v>
-      </c>
-      <c r="N4" t="s">
-        <v>82</v>
-      </c>
-      <c r="O4">
+        <v>187.6359537061866</v>
+      </c>
+      <c r="N4">
+        <v>210.2518800529839</v>
+      </c>
+      <c r="O4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4">
         <v>0.6960251889168766</v>
       </c>
-      <c r="P4">
-        <v>153.85164105967</v>
-      </c>
       <c r="Q4">
-        <v>168.0023224950234</v>
+        <v>153.8340149268989</v>
       </c>
       <c r="R4">
-        <v>188.8824715430559</v>
-      </c>
-      <c r="S4" t="s">
-        <v>87</v>
-      </c>
-      <c r="T4">
+        <v>167.9859676924651</v>
+      </c>
+      <c r="S4">
+        <v>188.8659646252943</v>
+      </c>
+      <c r="T4" t="s">
+        <v>104</v>
+      </c>
+      <c r="U4">
         <v>0.1970982367758186</v>
       </c>
-      <c r="U4">
-        <v>35.33696266970165</v>
-      </c>
       <c r="V4">
-        <v>56.06523378580447</v>
+        <v>35.33415036532595</v>
       </c>
       <c r="W4">
-        <v>39.03874434386037</v>
-      </c>
-      <c r="X4" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y4">
+        <v>56.06255008247128</v>
+      </c>
+      <c r="X4">
+        <v>39.03525807208774</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z4">
         <v>0.1068765743073048</v>
       </c>
-      <c r="Z4" t="s">
-        <v>93</v>
-      </c>
       <c r="AA4">
+        <v>299</v>
+      </c>
+      <c r="AB4">
+        <v>141</v>
+      </c>
+      <c r="AC4">
         <v>21082</v>
-      </c>
-      <c r="AB4">
-        <v>299</v>
-      </c>
-      <c r="AC4">
-        <v>141</v>
       </c>
       <c r="AD4">
         <v>2.120567375886525</v>
@@ -1116,62 +1125,62 @@
       <c r="J5">
         <v>-80.4095616039</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5">
         <v>171.6524343774405</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>186.0459767897252</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>209.8695459237344</v>
       </c>
-      <c r="N5" t="s">
-        <v>82</v>
-      </c>
-      <c r="O5">
+      <c r="O5" t="s">
+        <v>97</v>
+      </c>
+      <c r="P5">
         <v>0.5529653333333333</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>151.0872798556223</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>163.9499035409798</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>185.6025110461135</v>
       </c>
-      <c r="S5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T5">
+      <c r="T5" t="s">
+        <v>104</v>
+      </c>
+      <c r="U5">
         <v>0.3426986666666667</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>62.50738639268459</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>61.79379440779776</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>41.63170270407647</v>
       </c>
-      <c r="X5" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y5">
+      <c r="Y5" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z5">
         <v>0.104336</v>
       </c>
-      <c r="Z5" t="s">
-        <v>94</v>
-      </c>
       <c r="AA5">
+        <v>287</v>
+      </c>
+      <c r="AB5">
+        <v>226</v>
+      </c>
+      <c r="AC5">
         <v>19528.5</v>
-      </c>
-      <c r="AB5">
-        <v>287</v>
-      </c>
-      <c r="AC5">
-        <v>226</v>
       </c>
       <c r="AD5">
         <v>1.269911504424779</v>
@@ -1203,70 +1212,70 @@
         <v>38899</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
-      </c>
-      <c r="K6">
-        <v>122.6745064687805</v>
+        <v>83</v>
+      </c>
+      <c r="K6" t="s">
+        <v>88</v>
       </c>
       <c r="L6">
-        <v>133.2987529069956</v>
+        <v>122.6752668101727</v>
       </c>
       <c r="M6">
-        <v>155.9339800856488</v>
-      </c>
-      <c r="N6" t="s">
-        <v>81</v>
-      </c>
-      <c r="O6">
+        <v>133.2995499224752</v>
+      </c>
+      <c r="N6">
+        <v>155.9353107642291</v>
+      </c>
+      <c r="O6" t="s">
+        <v>99</v>
+      </c>
+      <c r="P6">
         <v>0.5690364025695932</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>153.8474315087378</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>166.3450154648808</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>197.2461172689396</v>
       </c>
-      <c r="S6" t="s">
-        <v>88</v>
-      </c>
-      <c r="T6">
+      <c r="T6" t="s">
+        <v>104</v>
+      </c>
+      <c r="U6">
         <v>0.3890835117773019</v>
       </c>
-      <c r="U6">
-        <v>52.66094069530308</v>
-      </c>
       <c r="V6">
-        <v>70.53609406952461</v>
+        <v>52.67208422774856</v>
       </c>
       <c r="W6">
-        <v>35.3840490797611</v>
-      </c>
-      <c r="X6" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y6">
+        <v>70.54451599713286</v>
+      </c>
+      <c r="X6">
+        <v>35.40294388225121</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z6">
         <v>0.04188008565310492</v>
       </c>
-      <c r="Z6" t="s">
-        <v>95</v>
-      </c>
       <c r="AA6">
+        <v>499</v>
+      </c>
+      <c r="AB6">
+        <v>456</v>
+      </c>
+      <c r="AC6">
         <v>227544</v>
-      </c>
-      <c r="AB6">
-        <v>499</v>
-      </c>
-      <c r="AC6">
-        <v>456</v>
       </c>
       <c r="AD6">
         <v>1.094298245614035</v>
@@ -1298,70 +1307,70 @@
         <v>38490</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7">
         <v>130.2153140167135</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>142.5762781447286</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>169.1631390723637</v>
       </c>
-      <c r="N7" t="s">
-        <v>81</v>
-      </c>
-      <c r="O7">
+      <c r="O7" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7">
         <v>0.5621128205128205</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>141.6161632228142</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>155.2422459042467</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>188.0124643926126</v>
       </c>
-      <c r="S7" t="s">
-        <v>87</v>
-      </c>
-      <c r="T7">
+      <c r="T7" t="s">
+        <v>104</v>
+      </c>
+      <c r="U7">
         <v>0.354651282051282</v>
       </c>
-      <c r="U7">
-        <v>55.74394676853434</v>
-      </c>
       <c r="V7">
+        <v>55.74394676853433</v>
+      </c>
+      <c r="W7">
         <v>73.41741112685592</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>52.70864395292821</v>
       </c>
-      <c r="X7" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y7">
+      <c r="Y7" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z7">
         <v>0.08323589743589743</v>
       </c>
-      <c r="Z7" t="s">
-        <v>96</v>
-      </c>
       <c r="AA7">
+        <v>216</v>
+      </c>
+      <c r="AB7">
+        <v>228</v>
+      </c>
+      <c r="AC7">
         <v>15944.5</v>
-      </c>
-      <c r="AB7">
-        <v>216</v>
-      </c>
-      <c r="AC7">
-        <v>228</v>
       </c>
       <c r="AD7">
         <v>0.9473684210526315</v>
@@ -1396,7 +1405,7 @@
         <v>36602</v>
       </c>
       <c r="H8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I8">
         <v>37.2504015</v>
@@ -1404,62 +1413,62 @@
       <c r="J8">
         <v>-80.66645370000001</v>
       </c>
-      <c r="K8">
+      <c r="K8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8">
         <v>221.8846870062522</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>218.1225171168326</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>213.5128846587863</v>
       </c>
-      <c r="N8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O8">
+      <c r="O8" t="s">
+        <v>100</v>
+      </c>
+      <c r="P8">
         <v>0.5656010638297873</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>53.75527160573193</v>
       </c>
-      <c r="Q8">
-        <v>90.61624284004093</v>
-      </c>
       <c r="R8">
-        <v>15.63931201610202</v>
-      </c>
-      <c r="S8" t="s">
-        <v>89</v>
-      </c>
-      <c r="T8">
+        <v>90.61624284004091</v>
+      </c>
+      <c r="S8">
+        <v>15.63931201610205</v>
+      </c>
+      <c r="T8" t="s">
+        <v>105</v>
+      </c>
+      <c r="U8">
         <v>0.3361010638297872</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>84.48962701390603</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>117.3242661664122</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>39.85019863164931</v>
       </c>
-      <c r="X8" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y8">
+      <c r="Y8" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z8">
         <v>0.09829787234042553</v>
       </c>
-      <c r="Z8" t="s">
-        <v>97</v>
-      </c>
       <c r="AA8">
+        <v>520</v>
+      </c>
+      <c r="AB8">
+        <v>519</v>
+      </c>
+      <c r="AC8">
         <v>80554.5</v>
-      </c>
-      <c r="AB8">
-        <v>520</v>
-      </c>
-      <c r="AC8">
-        <v>519</v>
       </c>
       <c r="AD8">
         <v>1.001926782273603</v>
@@ -1494,7 +1503,7 @@
         <v>36600</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I9">
         <v>37.2496022353</v>
@@ -1502,62 +1511,62 @@
       <c r="J9">
         <v>-80.66670543399999</v>
       </c>
-      <c r="K9">
-        <v>219.1904850983604</v>
+      <c r="K9" t="s">
+        <v>91</v>
       </c>
       <c r="L9">
+        <v>219.1904850983605</v>
+      </c>
+      <c r="M9">
         <v>217.7451419079183</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>217.2594449391349</v>
       </c>
-      <c r="N9" t="s">
-        <v>84</v>
-      </c>
-      <c r="O9">
+      <c r="O9" t="s">
+        <v>100</v>
+      </c>
+      <c r="P9">
         <v>0.7033315789473684</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>36.43909321616746</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>73.84828226202707</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>14.8097799325613</v>
       </c>
-      <c r="S9" t="s">
-        <v>89</v>
-      </c>
-      <c r="T9">
+      <c r="T9" t="s">
+        <v>103</v>
+      </c>
+      <c r="U9">
         <v>0.2779894736842105</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>132.5333333333334</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>149.3052039381153</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>120.4810126582273</v>
       </c>
-      <c r="X9" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y9">
+      <c r="Y9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z9">
         <v>0.01867894736842105</v>
       </c>
-      <c r="Z9" t="s">
-        <v>98</v>
-      </c>
       <c r="AA9">
+        <v>453</v>
+      </c>
+      <c r="AB9">
+        <v>454</v>
+      </c>
+      <c r="AC9">
         <v>54472</v>
-      </c>
-      <c r="AB9">
-        <v>453</v>
-      </c>
-      <c r="AC9">
-        <v>454</v>
       </c>
       <c r="AD9">
         <v>0.9977973568281938</v>
@@ -1592,7 +1601,7 @@
         <v>36600</v>
       </c>
       <c r="H10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I10">
         <v>37.2485728184</v>
@@ -1600,62 +1609,62 @@
       <c r="J10">
         <v>-80.66748366829999</v>
       </c>
-      <c r="K10">
+      <c r="K10" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10">
         <v>211.2274908387691</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>208.9123625816136</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>206.2215942323034</v>
       </c>
-      <c r="N10" t="s">
-        <v>85</v>
-      </c>
-      <c r="O10">
+      <c r="O10" t="s">
+        <v>101</v>
+      </c>
+      <c r="P10">
         <v>0.9008279569892473</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>26.55634178904509</v>
       </c>
-      <c r="Q10">
-        <v>64.45220293724373</v>
-      </c>
       <c r="R10">
+        <v>64.45220293724375</v>
+      </c>
+      <c r="S10">
         <v>8.518558077451559</v>
       </c>
-      <c r="S10" t="s">
-        <v>84</v>
-      </c>
-      <c r="T10">
+      <c r="T10" t="s">
+        <v>103</v>
+      </c>
+      <c r="U10">
         <v>0.0806505376344086</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>76.94748990190439</v>
       </c>
-      <c r="V10">
-        <v>105.7270628967121</v>
-      </c>
       <c r="W10">
+        <v>105.727062896712</v>
+      </c>
+      <c r="X10">
         <v>40.03923831505807</v>
       </c>
-      <c r="X10" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y10">
+      <c r="Y10" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z10">
         <v>0.01852150537634408</v>
       </c>
-      <c r="Z10" t="s">
-        <v>99</v>
-      </c>
       <c r="AA10">
+        <v>127</v>
+      </c>
+      <c r="AB10">
+        <v>355</v>
+      </c>
+      <c r="AC10">
         <v>45085</v>
-      </c>
-      <c r="AB10">
-        <v>127</v>
-      </c>
-      <c r="AC10">
-        <v>355</v>
       </c>
       <c r="AD10">
         <v>0.3577464788732395</v>
@@ -1690,7 +1699,7 @@
         <v>36600</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I11">
         <v>37.2504015</v>
@@ -1698,62 +1707,62 @@
       <c r="J11">
         <v>-80.66645370000001</v>
       </c>
-      <c r="K11">
+      <c r="K11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11">
         <v>214.5962834987609</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>210.341278400136</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>204.9647423905637</v>
       </c>
-      <c r="N11" t="s">
-        <v>85</v>
-      </c>
-      <c r="O11">
+      <c r="O11" t="s">
+        <v>101</v>
+      </c>
+      <c r="P11">
         <v>0.7428283378746594</v>
       </c>
-      <c r="P11">
-        <v>59.30306466135823</v>
-      </c>
       <c r="Q11">
-        <v>76.36402441058524</v>
+        <v>59.33412069998508</v>
       </c>
       <c r="R11">
-        <v>27.15283289426759</v>
-      </c>
-      <c r="S11" t="s">
-        <v>83</v>
-      </c>
-      <c r="T11">
-        <v>0.1651444141689373</v>
+        <v>76.39573491250984</v>
+      </c>
+      <c r="S11">
+        <v>27.18354514606449</v>
+      </c>
+      <c r="T11" t="s">
+        <v>105</v>
       </c>
       <c r="U11">
-        <v>84.39739565167143</v>
+        <v>0.1653079019073569</v>
       </c>
       <c r="V11">
-        <v>100.3088594349491</v>
+        <v>84.44690911213887</v>
       </c>
       <c r="W11">
-        <v>57.47093361237843</v>
-      </c>
-      <c r="X11" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y11">
-        <v>0.09202724795640327</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>100</v>
+        <v>100.3524604518122</v>
+      </c>
+      <c r="X11">
+        <v>57.54270036776209</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z11">
+        <v>0.09186376021798365</v>
       </c>
       <c r="AA11">
+        <v>391</v>
+      </c>
+      <c r="AB11">
+        <v>394</v>
+      </c>
+      <c r="AC11">
         <v>46800</v>
-      </c>
-      <c r="AB11">
-        <v>391</v>
-      </c>
-      <c r="AC11">
-        <v>394</v>
       </c>
       <c r="AD11">
         <v>0.9923857868020305</v>
@@ -1788,7 +1797,7 @@
         <v>36600</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I12">
         <v>37.2504015</v>
@@ -1796,62 +1805,62 @@
       <c r="J12">
         <v>-80.66645370000001</v>
       </c>
-      <c r="K12">
+      <c r="K12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L12">
         <v>201.4368865399079</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>199.816989106027</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>197.0657658629451</v>
       </c>
-      <c r="N12" t="s">
-        <v>86</v>
-      </c>
-      <c r="O12">
+      <c r="O12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P12">
         <v>0.5228820512820512</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>183.383432378895</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>182.4128819256855</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>180.6446605438499</v>
       </c>
-      <c r="S12" t="s">
-        <v>86</v>
-      </c>
-      <c r="T12">
+      <c r="T12" t="s">
+        <v>105</v>
+      </c>
+      <c r="U12">
         <v>0.4272615384615385</v>
       </c>
-      <c r="U12">
-        <v>60.54896111909838</v>
-      </c>
       <c r="V12">
+        <v>60.54896111909841</v>
+      </c>
+      <c r="W12">
         <v>73.46019337585025</v>
       </c>
-      <c r="W12">
-        <v>35.59031063568744</v>
-      </c>
-      <c r="X12" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y12">
+      <c r="X12">
+        <v>35.59031063568742</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z12">
         <v>0.04985641025641026</v>
       </c>
-      <c r="Z12" t="s">
-        <v>101</v>
-      </c>
       <c r="AA12">
-        <v>9634</v>
+        <v>171</v>
       </c>
       <c r="AB12">
         <v>171</v>
       </c>
       <c r="AC12">
-        <v>171</v>
+        <v>9634</v>
       </c>
       <c r="AD12">
         <v>1</v>
@@ -1886,7 +1895,7 @@
         <v>36660</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I13">
         <v>37.2504015</v>
@@ -1894,62 +1903,62 @@
       <c r="J13">
         <v>-80.66645370000001</v>
       </c>
-      <c r="K13">
+      <c r="K13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L13">
         <v>209.4411456859088</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>208.0204859488259</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>208.4494137937803</v>
       </c>
-      <c r="N13" t="s">
-        <v>85</v>
-      </c>
-      <c r="O13">
+      <c r="O13" t="s">
+        <v>103</v>
+      </c>
+      <c r="P13">
         <v>0.8300765027322404</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>41.01335407260117</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>67.53761523578665</v>
       </c>
-      <c r="R13">
-        <v>19.91608179370849</v>
-      </c>
-      <c r="S13" t="s">
-        <v>84</v>
-      </c>
-      <c r="T13">
+      <c r="S13">
+        <v>19.91608179370846</v>
+      </c>
+      <c r="T13" t="s">
+        <v>101</v>
+      </c>
+      <c r="U13">
         <v>0.1440382513661202</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>159.8989856297552</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>164.1223584108203</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>157.4387151310225</v>
       </c>
-      <c r="X13" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y13">
+      <c r="Y13" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z13">
         <v>0.02588524590163934</v>
       </c>
-      <c r="Z13" t="s">
-        <v>102</v>
-      </c>
       <c r="AA13">
+        <v>181</v>
+      </c>
+      <c r="AB13">
+        <v>262</v>
+      </c>
+      <c r="AC13">
         <v>47422</v>
-      </c>
-      <c r="AB13">
-        <v>181</v>
-      </c>
-      <c r="AC13">
-        <v>262</v>
       </c>
       <c r="AD13">
         <v>0.6908396946564885</v>
@@ -1984,70 +1993,70 @@
         <v>37380</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
-      </c>
-      <c r="K14">
-        <v>209.0773185863931</v>
+        <v>83</v>
+      </c>
+      <c r="K14" t="s">
+        <v>96</v>
       </c>
       <c r="L14">
-        <v>205.439694473329</v>
+        <v>209.0764199124769</v>
       </c>
       <c r="M14">
-        <v>200.4629688874748</v>
-      </c>
-      <c r="N14" t="s">
-        <v>85</v>
-      </c>
-      <c r="O14">
-        <v>0.9164659685863874</v>
+        <v>205.4390274556428</v>
+      </c>
+      <c r="N14">
+        <v>200.4619414325455</v>
+      </c>
+      <c r="O14" t="s">
+        <v>101</v>
       </c>
       <c r="P14">
-        <v>33.56708707901527</v>
+        <v>0.9164712041884817</v>
       </c>
       <c r="Q14">
-        <v>65.45679592111628</v>
+        <v>33.55626383948211</v>
       </c>
       <c r="R14">
-        <v>12.02287669394016</v>
-      </c>
-      <c r="S14" t="s">
-        <v>84</v>
-      </c>
-      <c r="T14">
-        <v>0.07803141361256545</v>
+        <v>65.45091592297919</v>
+      </c>
+      <c r="S14">
+        <v>12.01214520565472</v>
+      </c>
+      <c r="T14" t="s">
+        <v>103</v>
       </c>
       <c r="U14">
-        <v>127.1730038022816</v>
+        <v>0.07802617801047121</v>
       </c>
       <c r="V14">
-        <v>139.7186311787071</v>
+        <v>126.8972407231211</v>
       </c>
       <c r="W14">
-        <v>119.6492395437262</v>
-      </c>
-      <c r="X14" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y14">
+        <v>139.4509990485251</v>
+      </c>
+      <c r="X14">
+        <v>119.3577545195052</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z14">
         <v>0.005502617801047121</v>
       </c>
-      <c r="Z14" t="s">
-        <v>103</v>
-      </c>
       <c r="AA14">
+        <v>226</v>
+      </c>
+      <c r="AB14">
+        <v>230</v>
+      </c>
+      <c r="AC14">
         <v>15060.5</v>
-      </c>
-      <c r="AB14">
-        <v>226</v>
-      </c>
-      <c r="AC14">
-        <v>230</v>
       </c>
       <c r="AD14">
         <v>0.9826086956521739</v>

</xml_diff>

<commit_message>
update time observed at
</commit_message>
<xml_diff>
--- a/iNatStruct.xlsx
+++ b/iNatStruct.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="115">
   <si>
     <t>Image_Label</t>
   </si>
@@ -151,6 +151,9 @@
     <t>p13</t>
   </si>
   <si>
+    <t>p14</t>
+  </si>
+  <si>
     <t>https://inaturalist-open-data.s3.amazonaws.com/photos/203921715/medium.jpg</t>
   </si>
   <si>
@@ -190,6 +193,9 @@
     <t>https://inaturalist-open-data.s3.amazonaws.com/photos/204639334/medium.jpeg</t>
   </si>
   <si>
+    <t>https://inaturalist-open-data.s3.amazonaws.com/photos/205799198/medium.jpeg</t>
+  </si>
+  <si>
     <t>Carolina sweetshrub</t>
   </si>
   <si>
@@ -211,6 +217,9 @@
     <t>Sassafras</t>
   </si>
   <si>
+    <t>Striped Maple</t>
+  </si>
+  <si>
     <t>llhouse2</t>
   </si>
   <si>
@@ -253,6 +262,9 @@
     <t>10:23:00</t>
   </si>
   <si>
+    <t>10:32:00</t>
+  </si>
+  <si>
     <t>Highview Dr, Blacksburg, VA, US</t>
   </si>
   <si>
@@ -268,6 +280,9 @@
     <t>Giles County, VA, USA</t>
   </si>
   <si>
+    <t>Blacksburg, VA, USA</t>
+  </si>
+  <si>
     <t xml:space="preserve">             40.343137</t>
   </si>
   <si>
@@ -277,67 +292,70 @@
     <t>['#bccbdd', '#2a4b13', '#a3b2bd']</t>
   </si>
   <si>
-    <t>['#393117', '#b7c6db', '#5c6c44']</t>
+    <t>['#5c6c44', '#b7c6db', '#393117']</t>
   </si>
   <si>
     <t>['#9aa8bd', '#233827', '#adbcd2']</t>
   </si>
   <si>
-    <t>['#97a4ba', '#3f3e2a', '#acbad2']</t>
-  </si>
-  <si>
-    <t>['#7b859c', '#354723', '#9aa6c5']</t>
-  </si>
-  <si>
-    <t>['#828fa9', '#384935', '#8e9bbc']</t>
-  </si>
-  <si>
-    <t>['#dedad6', '#365b10', '#547528']</t>
-  </si>
-  <si>
-    <t>['#dbdad9', '#244a0f', '#859578']</t>
-  </si>
-  <si>
-    <t>['#d3d1ce', '#1b4009', '#4d6a28']</t>
-  </si>
-  <si>
-    <t>['#54643a', '#d7d2cd', '#3b4c1b']</t>
+    <t>['#97a4ba', '#acbad2', '#3f3e2a']</t>
+  </si>
+  <si>
+    <t>['#7b859c', '#9aa6c5', '#354723']</t>
+  </si>
+  <si>
+    <t>['#8e9bbc', '#384935', '#828fa9']</t>
+  </si>
+  <si>
+    <t>['#355a0f', '#dedad5', '#537426']</t>
+  </si>
+  <si>
+    <t>['#dbdad9', '#254a0f', '#87987d']</t>
+  </si>
+  <si>
+    <t>['#d3d1ce', '#4d6a28', '#1b4009']</t>
+  </si>
+  <si>
+    <t>['#546439', '#d7d2cd', '#3b4c1b']</t>
   </si>
   <si>
     <t>['#c9c8c5', '#3d4924', '#b7b6b5']</t>
   </si>
   <si>
-    <t>['#a0a49d', '#d1d0d0', '#294414']</t>
+    <t>['#d1d0d0', '#294414', '#a0a49d']</t>
   </si>
   <si>
     <t>['#d1cdc8', '#22410c', '#7f8b77']</t>
   </si>
   <si>
+    <t>['#d6d2d0', '#27470d', '#4e6b25']</t>
+  </si>
+  <si>
     <t>lightsteelblue</t>
   </si>
   <si>
+    <t>darkolivegreen</t>
+  </si>
+  <si>
+    <t>darkgray</t>
+  </si>
+  <si>
+    <t>lightslategray</t>
+  </si>
+  <si>
+    <t>gainsboro</t>
+  </si>
+  <si>
+    <t>lightgray</t>
+  </si>
+  <si>
+    <t>silver</t>
+  </si>
+  <si>
+    <t>darkgreen</t>
+  </si>
+  <si>
     <t>darkslategray</t>
-  </si>
-  <si>
-    <t>darkgray</t>
-  </si>
-  <si>
-    <t>lightslategray</t>
-  </si>
-  <si>
-    <t>gainsboro</t>
-  </si>
-  <si>
-    <t>lightgray</t>
-  </si>
-  <si>
-    <t>darkolivegreen</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
-    <t>darkgreen</t>
   </si>
   <si>
     <t>gray</t>
@@ -711,7 +729,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -820,22 +838,22 @@
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G2">
         <v>43641</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I2">
         <v>37.2463215678</v>
@@ -844,49 +862,49 @@
         <v>-80.40952306609999</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L2">
-        <v>188.3449388529327</v>
+        <v>188.3411619282971</v>
       </c>
       <c r="M2">
-        <v>202.8493173887958</v>
+        <v>202.8461486360588</v>
       </c>
       <c r="N2">
-        <v>220.9205257630685</v>
+        <v>220.9146163875584</v>
       </c>
       <c r="O2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="P2">
         <v>0.6489010989010989</v>
       </c>
       <c r="Q2">
-        <v>42.30201561223798</v>
+        <v>42.29772557790812</v>
       </c>
       <c r="R2">
-        <v>75.41505301175626</v>
+        <v>75.4116797166182</v>
       </c>
       <c r="S2">
-        <v>19.39219387159625</v>
+        <v>19.38616237881138</v>
       </c>
       <c r="T2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="U2">
         <v>0.2357857142857143</v>
       </c>
       <c r="V2">
-        <v>163.302203817412</v>
+        <v>163.2695718508634</v>
       </c>
       <c r="W2">
-        <v>178.0159455471465</v>
+        <v>177.9810241251073</v>
       </c>
       <c r="X2">
-        <v>189.2772145271066</v>
+        <v>189.2412033946783</v>
       </c>
       <c r="Y2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="Z2">
         <v>0.1153131868131868</v>
@@ -915,25 +933,25 @@
         <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G3">
         <v>43743</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I3">
         <v>37.3504969752</v>
@@ -942,52 +960,52 @@
         <v>-80.4847910049</v>
       </c>
       <c r="K3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L3">
-        <v>183.2364997904586</v>
+        <v>183.2323597318077</v>
       </c>
       <c r="M3">
-        <v>198.2781410869785</v>
+        <v>198.2738788032164</v>
       </c>
       <c r="N3">
-        <v>218.8874672824065</v>
+        <v>218.8811673730186</v>
       </c>
       <c r="O3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="P3">
-        <v>0.6690899470899471</v>
+        <v>0.6690952380952381</v>
       </c>
       <c r="Q3">
-        <v>57.40042536141196</v>
+        <v>57.38457028237269</v>
       </c>
       <c r="R3">
-        <v>48.61307523965405</v>
+        <v>48.57086869310589</v>
       </c>
       <c r="S3">
-        <v>22.78796658755505</v>
+        <v>22.76883197037648</v>
       </c>
       <c r="T3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="U3">
-        <v>0.1722698412698413</v>
+        <v>0.1721058201058201</v>
       </c>
       <c r="V3">
-        <v>92.18912812334153</v>
+        <v>92.14643295820761</v>
       </c>
       <c r="W3">
-        <v>107.7850544922935</v>
+        <v>107.7406632805519</v>
       </c>
       <c r="X3">
-        <v>67.624003189801</v>
+        <v>67.55924044750695</v>
       </c>
       <c r="Y3" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="Z3">
-        <v>0.1586402116402116</v>
+        <v>0.1587989417989418</v>
       </c>
       <c r="AA3">
         <v>428</v>
@@ -1013,22 +1031,22 @@
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G4">
         <v>43821</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I4">
         <v>37.2461629761</v>
@@ -1037,49 +1055,49 @@
         <v>-80.4092512154</v>
       </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="L4">
-        <v>172.7732299764028</v>
+        <v>172.7767881710603</v>
       </c>
       <c r="M4">
-        <v>187.6358839623083</v>
+        <v>187.6401065878875</v>
       </c>
       <c r="N4">
-        <v>210.2517768995839</v>
+        <v>210.2568825940269</v>
       </c>
       <c r="O4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="P4">
         <v>0.6960251889168766</v>
       </c>
       <c r="Q4">
-        <v>153.8308242811499</v>
+        <v>153.85164105967</v>
       </c>
       <c r="R4">
-        <v>167.9830031948883</v>
+        <v>168.0023224950234</v>
       </c>
       <c r="S4">
-        <v>188.8616996805116</v>
+        <v>188.8824715430559</v>
       </c>
       <c r="T4" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="U4">
         <v>0.1970982367758186</v>
       </c>
       <c r="V4">
-        <v>35.32824211570215</v>
+        <v>35.33696266970165</v>
       </c>
       <c r="W4">
-        <v>56.05699335311498</v>
+        <v>56.06523378580447</v>
       </c>
       <c r="X4">
-        <v>39.02866166969977</v>
+        <v>39.03874434386037</v>
       </c>
       <c r="Y4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="Z4">
         <v>0.1068765743073048</v>
@@ -1108,22 +1126,22 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G5">
         <v>43837</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I5">
         <v>37.2463788487</v>
@@ -1132,49 +1150,49 @@
         <v>-80.4095616039</v>
       </c>
       <c r="K5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L5">
-        <v>171.6524343774405</v>
+        <v>171.6508420301304</v>
       </c>
       <c r="M5">
-        <v>186.0459767897252</v>
+        <v>186.0440594918855</v>
       </c>
       <c r="N5">
-        <v>209.8695459237344</v>
+        <v>209.8676093288859</v>
       </c>
       <c r="O5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="P5">
         <v>0.5529653333333333</v>
       </c>
       <c r="Q5">
-        <v>151.0872798556223</v>
+        <v>151.08373793962</v>
       </c>
       <c r="R5">
-        <v>163.9499035409798</v>
+        <v>163.9463741051979</v>
       </c>
       <c r="S5">
-        <v>185.6025110461135</v>
+        <v>185.5980703392467</v>
       </c>
       <c r="T5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="U5">
         <v>0.3426986666666667</v>
       </c>
       <c r="V5">
-        <v>62.50738639268459</v>
+        <v>62.50506083223027</v>
       </c>
       <c r="W5">
-        <v>61.79379440779776</v>
+        <v>61.79112565176095</v>
       </c>
       <c r="X5">
-        <v>41.63170270407647</v>
+        <v>41.62810551067622</v>
       </c>
       <c r="Y5" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="Z5">
         <v>0.104336</v>
@@ -1203,43 +1221,43 @@
         <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G6">
         <v>38899</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L6">
-        <v>122.6754901591871</v>
+        <v>122.6745064687805</v>
       </c>
       <c r="M6">
-        <v>133.2997478643705</v>
+        <v>133.2987529069956</v>
       </c>
       <c r="N6">
-        <v>155.9358070221659</v>
+        <v>155.9339800856488</v>
       </c>
       <c r="O6" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="P6">
         <v>0.5690364025695932</v>
@@ -1254,22 +1272,22 @@
         <v>197.2461172689396</v>
       </c>
       <c r="T6" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="U6">
         <v>0.3890835117773019</v>
       </c>
       <c r="V6">
-        <v>52.67620605070157</v>
+        <v>52.6609406953031</v>
       </c>
       <c r="W6">
-        <v>70.54824202779545</v>
+        <v>70.53609406952461</v>
       </c>
       <c r="X6">
-        <v>35.40852412102041</v>
+        <v>35.3840490797611</v>
       </c>
       <c r="Y6" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="Z6">
         <v>0.04188008565310492</v>
@@ -1298,31 +1316,31 @@
         <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G7">
         <v>38490</v>
       </c>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="L7">
         <v>130.2153140167135</v>
@@ -1334,7 +1352,7 @@
         <v>169.1631390723637</v>
       </c>
       <c r="O7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="P7">
         <v>0.5621128205128205</v>
@@ -1349,7 +1367,7 @@
         <v>188.0124643926126</v>
       </c>
       <c r="T7" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="U7">
         <v>0.354651282051282</v>
@@ -1361,10 +1379,10 @@
         <v>73.41741112685592</v>
       </c>
       <c r="X7">
-        <v>52.70864395292821</v>
+        <v>52.70864395292823</v>
       </c>
       <c r="Y7" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="Z7">
         <v>0.08323589743589743</v>
@@ -1393,25 +1411,25 @@
         <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G8">
         <v>36602</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I8">
         <v>37.2504015</v>
@@ -1420,52 +1438,52 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="L8">
-        <v>221.883494780408</v>
+        <v>221.8705500705292</v>
       </c>
       <c r="M8">
-        <v>218.1215649393264</v>
+        <v>218.1109073812748</v>
       </c>
       <c r="N8">
-        <v>213.5111821687147</v>
+        <v>213.4954207804366</v>
       </c>
       <c r="O8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="P8">
-        <v>0.5656010638297873</v>
+        <v>0.5656914893617021</v>
       </c>
       <c r="Q8">
-        <v>53.74892947104929</v>
+        <v>53.21868375568248</v>
       </c>
       <c r="R8">
-        <v>90.61045340048679</v>
+        <v>90.09120112185622</v>
       </c>
       <c r="S8">
-        <v>15.63301322416959</v>
+        <v>15.28041939795983</v>
       </c>
       <c r="T8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="U8">
-        <v>0.3358510638297872</v>
+        <v>0.32725</v>
       </c>
       <c r="V8">
-        <v>84.45625344352797</v>
+        <v>82.6738338909678</v>
       </c>
       <c r="W8">
-        <v>117.2977961432537</v>
+        <v>115.9402184609364</v>
       </c>
       <c r="X8">
-        <v>39.82573002754887</v>
+        <v>38.18957882306889</v>
       </c>
       <c r="Y8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Z8">
-        <v>0.09854787234042553</v>
+        <v>0.1070585106382979</v>
       </c>
       <c r="AA8">
         <v>520</v>
@@ -1491,25 +1509,25 @@
         <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G9">
         <v>36600</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I9">
         <v>37.2496022353</v>
@@ -1518,52 +1536,52 @@
         <v>-80.66670543399999</v>
       </c>
       <c r="K9" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="L9">
-        <v>219.1904850983604</v>
+        <v>219.231094734163</v>
       </c>
       <c r="M9">
-        <v>217.7451419079183</v>
+        <v>217.7756083312731</v>
       </c>
       <c r="N9">
-        <v>217.2594449391349</v>
+        <v>217.3014731765101</v>
       </c>
       <c r="O9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="P9">
-        <v>0.7033315789473684</v>
+        <v>0.7028</v>
       </c>
       <c r="Q9">
-        <v>36.43909321616746</v>
+        <v>36.57267007991675</v>
       </c>
       <c r="R9">
-        <v>73.84828226202707</v>
+        <v>73.96176153859845</v>
       </c>
       <c r="S9">
-        <v>14.8097799325613</v>
+        <v>14.91364228900076</v>
       </c>
       <c r="T9" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="U9">
-        <v>0.2779894736842105</v>
+        <v>0.2784947368421052</v>
       </c>
       <c r="V9">
-        <v>132.5333333333334</v>
+        <v>135.4859075535513</v>
       </c>
       <c r="W9">
-        <v>149.3052039381153</v>
+        <v>151.5625704622322</v>
       </c>
       <c r="X9">
-        <v>120.4810126582273</v>
+        <v>124.5197294250277</v>
       </c>
       <c r="Y9" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="Z9">
-        <v>0.01867894736842105</v>
+        <v>0.01870526315789474</v>
       </c>
       <c r="AA9">
         <v>453</v>
@@ -1589,25 +1607,25 @@
         <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G10">
         <v>36600</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I10">
         <v>37.2485728184</v>
@@ -1616,7 +1634,7 @@
         <v>-80.66748366829999</v>
       </c>
       <c r="K10" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="L10">
         <v>211.2274908387691</v>
@@ -1628,7 +1646,7 @@
         <v>206.2215942323034</v>
       </c>
       <c r="O10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="P10">
         <v>0.9008279569892473</v>
@@ -1643,22 +1661,22 @@
         <v>8.518558077451559</v>
       </c>
       <c r="T10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U10">
         <v>0.0806505376344086</v>
       </c>
       <c r="V10">
-        <v>76.9474899019044</v>
+        <v>76.94748990190439</v>
       </c>
       <c r="W10">
-        <v>105.7270628967121</v>
+        <v>105.727062896712</v>
       </c>
       <c r="X10">
         <v>40.03923831505807</v>
       </c>
       <c r="Y10" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="Z10">
         <v>0.01852150537634408</v>
@@ -1687,25 +1705,25 @@
         <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G11">
         <v>36600</v>
       </c>
       <c r="H11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I11">
         <v>37.2504015</v>
@@ -1714,52 +1732,52 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K11" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L11">
-        <v>214.5962834987609</v>
+        <v>214.5946931349648</v>
       </c>
       <c r="M11">
-        <v>210.341278400136</v>
+        <v>210.3399724166332</v>
       </c>
       <c r="N11">
-        <v>204.9647423905637</v>
+        <v>204.9633199818077</v>
       </c>
       <c r="O11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P11">
         <v>0.7428283378746594</v>
       </c>
       <c r="Q11">
-        <v>59.31858908170905</v>
+        <v>59.26934518835945</v>
       </c>
       <c r="R11">
-        <v>76.38074143157648</v>
+        <v>76.3355282949567</v>
       </c>
       <c r="S11">
-        <v>27.16807114546862</v>
+        <v>27.12290670857382</v>
       </c>
       <c r="T11" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="U11">
-        <v>0.1651880108991826</v>
+        <v>0.1650681198910082</v>
       </c>
       <c r="V11">
-        <v>84.42287079110166</v>
+        <v>84.34402686895898</v>
       </c>
       <c r="W11">
-        <v>100.3298380519629</v>
+        <v>100.2523597197287</v>
       </c>
       <c r="X11">
-        <v>57.50786438309058</v>
+        <v>57.38548844751489</v>
       </c>
       <c r="Y11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Z11">
-        <v>0.09198365122615804</v>
+        <v>0.09210354223433243</v>
       </c>
       <c r="AA11">
         <v>391</v>
@@ -1785,25 +1803,25 @@
         <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G12">
         <v>36600</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I12">
         <v>37.2504015</v>
@@ -1812,40 +1830,40 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K12" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="L12">
-        <v>201.4368865399079</v>
+        <v>201.4001542546904</v>
       </c>
       <c r="M12">
-        <v>199.816989106027</v>
+        <v>199.7830964189475</v>
       </c>
       <c r="N12">
-        <v>197.0657658629451</v>
+        <v>197.0220447533949</v>
       </c>
       <c r="O12" t="s">
+        <v>111</v>
+      </c>
+      <c r="P12">
+        <v>0.5229897435897436</v>
+      </c>
+      <c r="Q12">
+        <v>183.3318768859392</v>
+      </c>
+      <c r="R12">
+        <v>182.3613035606515</v>
+      </c>
+      <c r="S12">
+        <v>180.6105129752562</v>
+      </c>
+      <c r="T12" t="s">
         <v>106</v>
       </c>
-      <c r="P12">
-        <v>0.5228820512820512</v>
-      </c>
-      <c r="Q12">
-        <v>183.383432378895</v>
-      </c>
-      <c r="R12">
-        <v>182.4128819256855</v>
-      </c>
-      <c r="S12">
-        <v>180.6446605438499</v>
-      </c>
-      <c r="T12" t="s">
-        <v>105</v>
-      </c>
       <c r="U12">
-        <v>0.4272615384615385</v>
+        <v>0.4271538461538462</v>
       </c>
       <c r="V12">
-        <v>60.54896111909841</v>
+        <v>60.54896111909838</v>
       </c>
       <c r="W12">
         <v>73.46019337585025</v>
@@ -1854,7 +1872,7 @@
         <v>35.59031063568744</v>
       </c>
       <c r="Y12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="Z12">
         <v>0.04985641025641026</v>
@@ -1883,25 +1901,25 @@
         <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G13">
         <v>36660</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I13">
         <v>37.2504015</v>
@@ -1910,22 +1928,22 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K13" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="L13">
-        <v>209.4411456859088</v>
+        <v>209.4418514324884</v>
       </c>
       <c r="M13">
-        <v>208.0204859488259</v>
+        <v>208.0211778491691</v>
       </c>
       <c r="N13">
-        <v>208.4494137937803</v>
+        <v>208.4503897198189</v>
       </c>
       <c r="O13" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="P13">
-        <v>0.8300765027322404</v>
+        <v>0.8296557377049181</v>
       </c>
       <c r="Q13">
         <v>41.01335407260117</v>
@@ -1934,28 +1952,28 @@
         <v>67.53761523578665</v>
       </c>
       <c r="S13">
-        <v>19.91608179370846</v>
+        <v>19.91608179370849</v>
       </c>
       <c r="T13" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="U13">
         <v>0.1440382513661202</v>
       </c>
       <c r="V13">
-        <v>159.8989856297552</v>
+        <v>159.928646822884</v>
       </c>
       <c r="W13">
-        <v>164.1223584108203</v>
+        <v>164.1465062275705</v>
       </c>
       <c r="X13">
-        <v>157.4387151310225</v>
+        <v>157.461262402364</v>
       </c>
       <c r="Y13" t="s">
         <v>107</v>
       </c>
       <c r="Z13">
-        <v>0.02588524590163934</v>
+        <v>0.02630601092896175</v>
       </c>
       <c r="AA13">
         <v>181</v>
@@ -1981,34 +1999,34 @@
         <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G14">
         <v>37380</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I14" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K14" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="L14">
         <v>209.0764199124769</v>
@@ -2020,37 +2038,37 @@
         <v>200.4619414325455</v>
       </c>
       <c r="O14" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="P14">
         <v>0.9164712041884817</v>
       </c>
       <c r="Q14">
-        <v>33.55234196750783</v>
+        <v>33.55626383948209</v>
       </c>
       <c r="R14">
-        <v>65.4481277680955</v>
+        <v>65.45091592297919</v>
       </c>
       <c r="S14">
-        <v>12.00946181719718</v>
+        <v>12.01214520565472</v>
       </c>
       <c r="T14" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="U14">
         <v>0.07802617801047121</v>
       </c>
       <c r="V14">
-        <v>126.8640684410649</v>
+        <v>126.8972407231211</v>
       </c>
       <c r="W14">
-        <v>139.4201520912546</v>
+        <v>139.4509990485251</v>
       </c>
       <c r="X14">
-        <v>119.2937262357414</v>
+        <v>119.3577545195052</v>
       </c>
       <c r="Y14" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="Z14">
         <v>0.005502617801047121</v>
@@ -2072,6 +2090,104 @@
       </c>
       <c r="AF14">
         <v>0.7597871052366058</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15">
+        <v>37920</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15">
+        <v>37.2295733</v>
+      </c>
+      <c r="J15">
+        <v>-80.4139393</v>
+      </c>
+      <c r="K15" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15">
+        <v>214.1140382334292</v>
+      </c>
+      <c r="M15">
+        <v>210.4988207221882</v>
+      </c>
+      <c r="N15">
+        <v>208.0128203359766</v>
+      </c>
+      <c r="O15" t="s">
+        <v>110</v>
+      </c>
+      <c r="P15">
+        <v>0.7513160621761658</v>
+      </c>
+      <c r="Q15">
+        <v>39.31901555607033</v>
+      </c>
+      <c r="R15">
+        <v>70.88771186439894</v>
+      </c>
+      <c r="S15">
+        <v>12.71705943810136</v>
+      </c>
+      <c r="T15" t="s">
+        <v>112</v>
+      </c>
+      <c r="U15">
+        <v>0.1782227979274612</v>
+      </c>
+      <c r="V15">
+        <v>78.42584933530279</v>
+      </c>
+      <c r="W15">
+        <v>107.3371491875899</v>
+      </c>
+      <c r="X15">
+        <v>37.0153618906978</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z15">
+        <v>0.07046113989637305</v>
+      </c>
+      <c r="AA15">
+        <v>290</v>
+      </c>
+      <c r="AB15">
+        <v>455</v>
+      </c>
+      <c r="AC15">
+        <v>47232.5</v>
+      </c>
+      <c r="AD15">
+        <v>0.6373626373626373</v>
+      </c>
+      <c r="AE15">
+        <v>0.4894458145945162</v>
+      </c>
+      <c r="AF15">
+        <v>0.7729284796714041</v>
       </c>
     </row>
   </sheetData>
@@ -2089,6 +2205,7 @@
     <hyperlink ref="B12" r:id="rId11"/>
     <hyperlink ref="B13" r:id="rId12"/>
     <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Jubilee: Update size feature
</commit_message>
<xml_diff>
--- a/iNatStruct.xlsx
+++ b/iNatStruct.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="114">
   <si>
     <t>Image_Label</t>
   </si>
@@ -112,6 +112,9 @@
     <t>Solidity</t>
   </si>
   <si>
+    <t>Angle</t>
+  </si>
+  <si>
     <t>p1</t>
   </si>
   <si>
@@ -289,46 +292,46 @@
     <t xml:space="preserve">             74.655070</t>
   </si>
   <si>
-    <t>['#2e5013', '#1d3e0d', '#47672e']</t>
-  </si>
-  <si>
-    <t>['#606e47', '#374e1c', '#411b17']</t>
-  </si>
-  <si>
-    <t>['#213625', '#2f4330', '#637372']</t>
-  </si>
-  <si>
-    <t>['#4b4831', '#303120', '#6d716b']</t>
+    <t>['#20410e', '#325316', '#52703e']</t>
+  </si>
+  <si>
+    <t>['#526335', '#392c16', '#7e8377']</t>
+  </si>
+  <si>
+    <t>['#213625', '#2d412e', '#60716e']</t>
+  </si>
+  <si>
+    <t>['#313221', '#4c4932', '#737876']</t>
   </si>
   <si>
     <t>['#7e89a3', '#727c8c', '#334521']</t>
   </si>
   <si>
-    <t>['#394b36', '#30422e', '#485a45']</t>
-  </si>
-  <si>
-    <t>['#3c6014', '#2b5009', '#567628']</t>
-  </si>
-  <si>
-    <t>['#1e450b', '#426423', '#a9b29f']</t>
-  </si>
-  <si>
-    <t>['#193f08', '#3e6018', '#70855a']</t>
-  </si>
-  <si>
-    <t>['#394a18', '#4d5e2f', '#7b846d']</t>
-  </si>
-  <si>
-    <t>['#33401b', '#46532c', '#727a67']</t>
-  </si>
-  <si>
-    <t>['#233e10', '#39521f', '#778578']</t>
-  </si>
-  <si>
-    <t>['#1d3e09', '#2f4c16', '#6d7e63']</t>
-  </si>
-  <si>
-    <t>['#27460d', '#48661e', '#7a8964']</t>
+    <t>['#394b36', '#31422e', '#485a44']</t>
+  </si>
+  <si>
+    <t>['#30550c', '#426618', '#617e33']</t>
+  </si>
+  <si>
+    <t>['#1f450b', '#426322', '#a7b09d']</t>
+  </si>
+  <si>
+    <t>['#183e08', '#395b14', '#637b43']</t>
+  </si>
+  <si>
+    <t>['#384918', '#4c5d2f', '#79826a']</t>
+  </si>
+  <si>
+    <t>['#32401a', '#46532b', '#717a66']</t>
+  </si>
+  <si>
+    <t>['#223d0f', '#37501d', '#758274']</t>
+  </si>
+  <si>
+    <t>['#1d3e09', '#2e4b15', '#6c7c61']</t>
+  </si>
+  <si>
+    <t>['#27460d', '#48661e', '#798961']</t>
   </si>
   <si>
     <t>darkgreen</t>
@@ -346,16 +349,13 @@
     <t>slategray</t>
   </si>
   <si>
-    <t>maroon</t>
+    <t>gray</t>
   </si>
   <si>
     <t>dimgray</t>
   </si>
   <si>
     <t>darkgray</t>
-  </si>
-  <si>
-    <t>gray</t>
   </si>
 </sst>
 </file>
@@ -726,13 +726,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF15"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,28 +829,31 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G2">
         <v>43641</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I2">
         <v>37.2463215678</v>
@@ -859,96 +862,99 @@
         <v>-80.40952306609999</v>
       </c>
       <c r="K2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L2">
-        <v>45.97814836112708</v>
+        <v>32.00785769379127</v>
       </c>
       <c r="M2">
-        <v>79.56411730879816</v>
+        <v>64.96418241419161</v>
       </c>
       <c r="N2">
-        <v>19.43789534215066</v>
+        <v>14.21635171615906</v>
       </c>
       <c r="O2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P2">
-        <v>0.5463167437643832</v>
+        <v>0.4822055370882633</v>
       </c>
       <c r="Q2">
-        <v>29.27318355640535</v>
+        <v>49.87979788164434</v>
       </c>
       <c r="R2">
-        <v>61.88121414913958</v>
+        <v>83.36186959479139</v>
       </c>
       <c r="S2">
-        <v>13.46534416826004</v>
+        <v>21.86060635506763</v>
       </c>
       <c r="T2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="U2">
-        <v>0.3745786745391571</v>
+        <v>0.478555986889514</v>
       </c>
       <c r="V2">
-        <v>71.14808362369338</v>
+        <v>82.48552864737161</v>
       </c>
       <c r="W2">
-        <v>102.7508710801394</v>
+        <v>111.8133490844655</v>
       </c>
       <c r="X2">
-        <v>46.02003484320558</v>
+        <v>61.50502067336102</v>
       </c>
       <c r="Y2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Z2">
-        <v>0.0791045816964597</v>
+        <v>0.03923847602222274</v>
       </c>
       <c r="AA2">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="AB2">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="AC2">
         <v>42647</v>
       </c>
       <c r="AD2">
-        <v>1.0187265917603</v>
+        <v>1.049586776859504</v>
       </c>
       <c r="AE2">
-        <v>0.7050139690201849</v>
+        <v>0.6938081603435934</v>
       </c>
       <c r="AF2">
         <v>0.9190767639325891</v>
       </c>
+      <c r="AG2">
+        <v>105.9358596801758</v>
+      </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3">
         <v>43743</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I3">
         <v>37.3504969752</v>
@@ -957,93 +963,96 @@
         <v>-80.4847910049</v>
       </c>
       <c r="K3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3">
-        <v>95.9524976437323</v>
+        <v>82.44866255144072</v>
       </c>
       <c r="M3">
-        <v>110.2499528746466</v>
+        <v>99.45085733882124</v>
       </c>
       <c r="N3">
-        <v>70.85183788878417</v>
+        <v>52.7458161865576</v>
       </c>
       <c r="O3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P3">
-        <v>0.3954607068469601</v>
+        <v>0.4818990313088901</v>
       </c>
       <c r="Q3">
-        <v>55.08265582655827</v>
+        <v>57.26036341927487</v>
       </c>
       <c r="R3">
-        <v>77.52032520325203</v>
+        <v>43.91903287190843</v>
       </c>
       <c r="S3">
-        <v>28.02484191508582</v>
+        <v>21.70807059438245</v>
       </c>
       <c r="T3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="U3">
-        <v>0.331933745495421</v>
+        <v>0.4434654676496843</v>
       </c>
       <c r="V3">
-        <v>65.05141100866163</v>
+        <v>126.394881976616</v>
       </c>
       <c r="W3">
-        <v>26.80441464096117</v>
+        <v>131.2717846900509</v>
       </c>
       <c r="X3">
-        <v>22.63704945515507</v>
+        <v>119.2565629825732</v>
       </c>
       <c r="Y3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Z3">
-        <v>0.272605547657619</v>
+        <v>0.07463550104142559</v>
       </c>
       <c r="AA3">
-        <v>428</v>
+        <v>374</v>
       </c>
       <c r="AB3">
-        <v>465</v>
+        <v>345</v>
       </c>
       <c r="AC3">
         <v>60445</v>
       </c>
       <c r="AD3">
-        <v>0.9204301075268817</v>
+        <v>1.084057971014493</v>
       </c>
       <c r="AE3">
-        <v>0.4723446486621655</v>
+        <v>0.4684569479965899</v>
       </c>
       <c r="AF3">
         <v>0.6568537958314317</v>
       </c>
+      <c r="AG3">
+        <v>46.17789459228516</v>
+      </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G4">
         <v>43821</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I4">
         <v>37.2461629761</v>
@@ -1052,93 +1061,96 @@
         <v>-80.4092512154</v>
       </c>
       <c r="K4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L4">
-        <v>33.08536082474227</v>
+        <v>32.69142990218924</v>
       </c>
       <c r="M4">
-        <v>53.92420618556701</v>
+        <v>53.51251746623188</v>
       </c>
       <c r="N4">
-        <v>37.13632989690721</v>
+        <v>36.8965999068468</v>
       </c>
       <c r="O4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P4">
-        <v>0.8377406092319193</v>
+        <v>0.802420108390955</v>
       </c>
       <c r="Q4">
-        <v>46.87076923076921</v>
+        <v>44.57684265551495</v>
       </c>
       <c r="R4">
-        <v>67.18358974358972</v>
+        <v>65.10663878724515</v>
       </c>
       <c r="S4">
-        <v>47.68358974358974</v>
+        <v>45.50888656560375</v>
       </c>
       <c r="T4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U4">
-        <v>0.1443188189123528</v>
+        <v>0.1787516352083723</v>
       </c>
       <c r="V4">
-        <v>99.24137931034483</v>
+        <v>96.38557213930358</v>
       </c>
       <c r="W4">
-        <v>115.3256704980843</v>
+        <v>112.9875621890547</v>
       </c>
       <c r="X4">
-        <v>114.1494252873563</v>
+        <v>110.2960199004975</v>
       </c>
       <c r="Y4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z4">
-        <v>0.0179405718557279</v>
+        <v>0.01882825640067277</v>
       </c>
       <c r="AA4">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="AB4">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="AC4">
         <v>21082</v>
       </c>
       <c r="AD4">
-        <v>2.120567375886525</v>
+        <v>2.478991596638656</v>
       </c>
       <c r="AE4">
-        <v>0.6181679568379076</v>
+        <v>0.6005412334425295</v>
       </c>
       <c r="AF4">
         <v>0.8983105013102669</v>
       </c>
+      <c r="AG4">
+        <v>89.91668701171875</v>
+      </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G5">
         <v>43837</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I5">
         <v>37.2463788487</v>
@@ -1147,286 +1159,295 @@
         <v>-80.4095616039</v>
       </c>
       <c r="K5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L5">
-        <v>74.59150057651128</v>
+        <v>49.08198207271602</v>
       </c>
       <c r="M5">
-        <v>72.10772525119421</v>
+        <v>50.01510726155686</v>
       </c>
       <c r="N5">
-        <v>48.63482128150223</v>
+        <v>32.56742874408293</v>
       </c>
       <c r="O5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P5">
-        <v>0.4851644753412926</v>
+        <v>0.500176313535842</v>
       </c>
       <c r="Q5">
-        <v>48.29093440055681</v>
+        <v>75.93321881039293</v>
       </c>
       <c r="R5">
-        <v>49.33252131546895</v>
+        <v>73.36772600386523</v>
       </c>
       <c r="S5">
-        <v>32.10875239255263</v>
+        <v>49.87889199055191</v>
       </c>
       <c r="T5" t="s">
         <v>107</v>
       </c>
       <c r="U5">
-        <v>0.4782126844995214</v>
+        <v>0.4691955065236008</v>
       </c>
       <c r="V5">
-        <v>109.4808510638298</v>
+        <v>115.1134868421052</v>
       </c>
       <c r="W5">
-        <v>112.6191489361702</v>
+        <v>119.5723684210526</v>
       </c>
       <c r="X5">
-        <v>107.4170212765957</v>
+        <v>118.4901315789474</v>
       </c>
       <c r="Y5" t="s">
         <v>111</v>
       </c>
       <c r="Z5">
-        <v>0.03662284015918593</v>
+        <v>0.03062817994055715</v>
       </c>
       <c r="AA5">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="AB5">
-        <v>226</v>
+        <v>152</v>
       </c>
       <c r="AC5">
         <v>19528.5</v>
       </c>
       <c r="AD5">
-        <v>1.269911504424779</v>
+        <v>1.756578947368421</v>
       </c>
       <c r="AE5">
-        <v>0.4927208962002321</v>
+        <v>0.4811871673565937</v>
       </c>
       <c r="AF5">
         <v>0.741386837759344</v>
       </c>
+      <c r="AG5">
+        <v>83.74250793457031</v>
+      </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G6">
         <v>38899</v>
       </c>
       <c r="H6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L6">
-        <v>126.0449522102748</v>
+        <v>125.8731294821853</v>
       </c>
       <c r="M6">
-        <v>137.0162783751494</v>
+        <v>136.8333474504473</v>
       </c>
       <c r="N6">
-        <v>163.2979390681004</v>
+        <v>163.1228189056415</v>
       </c>
       <c r="O6" t="s">
+        <v>109</v>
+      </c>
+      <c r="P6">
+        <v>0.5533310941173714</v>
+      </c>
+      <c r="Q6">
+        <v>113.5558440470702</v>
+      </c>
+      <c r="R6">
+        <v>123.6226391389919</v>
+      </c>
+      <c r="S6">
+        <v>139.7157334896777</v>
+      </c>
+      <c r="T6" t="s">
+        <v>110</v>
+      </c>
+      <c r="U6">
+        <v>0.3730637942212606</v>
+      </c>
+      <c r="V6">
+        <v>51.19274424525621</v>
+      </c>
+      <c r="W6">
+        <v>69.36353028534811</v>
+      </c>
+      <c r="X6">
+        <v>33.47268484140375</v>
+      </c>
+      <c r="Y6" t="s">
         <v>108</v>
       </c>
-      <c r="P6">
-        <v>0.5529952117230766</v>
-      </c>
-      <c r="Q6">
-        <v>113.5908115070846</v>
-      </c>
-      <c r="R6">
-        <v>123.6835551738944</v>
-      </c>
-      <c r="S6">
-        <v>139.900601116359</v>
-      </c>
-      <c r="T6" t="s">
-        <v>109</v>
-      </c>
-      <c r="U6">
-        <v>0.373454355144859</v>
-      </c>
-      <c r="V6">
-        <v>50.69700214132762</v>
-      </c>
-      <c r="W6">
-        <v>69.00428265524627</v>
-      </c>
-      <c r="X6">
-        <v>32.83297644539615</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>107</v>
-      </c>
       <c r="Z6">
-        <v>0.07355043313206427</v>
+        <v>0.07360511166136806</v>
       </c>
       <c r="AA6">
         <v>499</v>
       </c>
       <c r="AB6">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AC6">
-        <v>227544</v>
+        <v>126945.5</v>
       </c>
       <c r="AD6">
-        <v>1.094298245614035</v>
+        <v>1.089519650655022</v>
       </c>
       <c r="AE6">
-        <v>227544</v>
+        <v>0.5554580777275074</v>
       </c>
       <c r="AF6">
-        <v>0</v>
+        <v>0.7743199680379641</v>
+      </c>
+      <c r="AG6">
+        <v>63.34011459350586</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G7">
         <v>38490</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L7">
-        <v>57.04837443065809</v>
+        <v>57.28499114148319</v>
       </c>
       <c r="M7">
-        <v>74.68540914088271</v>
+        <v>74.96583143507972</v>
       </c>
       <c r="N7">
-        <v>53.8041463797707</v>
+        <v>54.02417109592508</v>
       </c>
       <c r="O7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P7">
-        <v>0.498578140454995</v>
+        <v>0.4885014836795252</v>
       </c>
       <c r="Q7">
-        <v>48.34974267173864</v>
+        <v>48.69292706030945</v>
       </c>
       <c r="R7">
-        <v>65.78496307898858</v>
+        <v>66.13688032838641</v>
       </c>
       <c r="S7">
-        <v>45.73797270082792</v>
+        <v>46.01720871487225</v>
       </c>
       <c r="T7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U7">
-        <v>0.3814910979228487</v>
+        <v>0.3915677546983185</v>
       </c>
       <c r="V7">
-        <v>71.99931129476585</v>
+        <v>71.8113402061856</v>
       </c>
       <c r="W7">
-        <v>90.39393939393938</v>
+        <v>90.21494845360823</v>
       </c>
       <c r="X7">
-        <v>68.64669421487604</v>
+        <v>68.46855670103103</v>
       </c>
       <c r="Y7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Z7">
         <v>0.1199307616221563</v>
       </c>
       <c r="AA7">
-        <v>216</v>
+        <v>132</v>
       </c>
       <c r="AB7">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="AC7">
         <v>15944.5</v>
       </c>
       <c r="AD7">
-        <v>0.9473684210526315</v>
+        <v>0.559322033898305</v>
       </c>
       <c r="AE7">
-        <v>0.6242463393626184</v>
+        <v>0.5118290960451978</v>
       </c>
       <c r="AF7">
         <v>0.961902750965251</v>
       </c>
+      <c r="AG7">
+        <v>3.063427686691284</v>
+      </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G8">
         <v>36602</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I8">
         <v>37.2504015</v>
@@ -1435,96 +1456,99 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L8">
-        <v>59.8522209567198</v>
+        <v>48.22573214873302</v>
       </c>
       <c r="M8">
-        <v>96.46568906605923</v>
+        <v>85.40270922452594</v>
       </c>
       <c r="N8">
-        <v>19.56947608200455</v>
+        <v>12.27149829987851</v>
       </c>
       <c r="O8" t="s">
         <v>106</v>
       </c>
       <c r="P8">
-        <v>0.5563202828237241</v>
+        <v>0.4571815412388582</v>
       </c>
       <c r="Q8">
-        <v>42.78999999999998</v>
+        <v>66.09947236878654</v>
       </c>
       <c r="R8">
-        <v>80.23206896551723</v>
+        <v>102.4359344626493</v>
       </c>
       <c r="S8">
-        <v>9.143103448275861</v>
+        <v>23.85592890863636</v>
       </c>
       <c r="T8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="U8">
-        <v>0.2699612621760878</v>
+        <v>0.4511264056564745</v>
       </c>
       <c r="V8">
-        <v>85.52622673434855</v>
+        <v>96.50637947592256</v>
       </c>
       <c r="W8">
-        <v>118.0833333333333</v>
+        <v>125.7557964055427</v>
       </c>
       <c r="X8">
-        <v>40.42554991539763</v>
+        <v>50.51173000411519</v>
       </c>
       <c r="Y8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Z8">
-        <v>0.173718455000188</v>
+        <v>0.09169205310466734</v>
       </c>
       <c r="AA8">
-        <v>520</v>
+        <v>362</v>
       </c>
       <c r="AB8">
-        <v>519</v>
+        <v>453</v>
       </c>
       <c r="AC8">
         <v>80554.5</v>
       </c>
       <c r="AD8">
-        <v>1.001926782273603</v>
+        <v>0.7991169977924945</v>
       </c>
       <c r="AE8">
-        <v>0.5129716305282261</v>
+        <v>0.4912279096996085</v>
       </c>
       <c r="AF8">
         <v>0.7763765336314659</v>
       </c>
+      <c r="AG8">
+        <v>127.713134765625</v>
+      </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G9">
         <v>36600</v>
       </c>
       <c r="H9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I9">
         <v>37.2496022353</v>
@@ -1533,96 +1557,99 @@
         <v>-80.66670543399999</v>
       </c>
       <c r="K9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L9">
-        <v>30.48150122614352</v>
+        <v>30.5734663412542</v>
       </c>
       <c r="M9">
-        <v>68.68130930802859</v>
+        <v>68.71120536454767</v>
       </c>
       <c r="N9">
-        <v>11.19746241603583</v>
+        <v>11.2331587801807</v>
       </c>
       <c r="O9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P9">
-        <v>0.7729343587126872</v>
+        <v>0.7691256332689433</v>
       </c>
       <c r="Q9">
-        <v>66.10406189555127</v>
+        <v>65.56579185520285</v>
       </c>
       <c r="R9">
-        <v>99.64835589941973</v>
+        <v>99.12787330316644</v>
       </c>
       <c r="S9">
-        <v>34.96711798839458</v>
+        <v>34.39683257918497</v>
       </c>
       <c r="T9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U9">
-        <v>0.1980901702081131</v>
+        <v>0.2013339650836462</v>
       </c>
       <c r="V9">
-        <v>169.25</v>
+        <v>166.726095003084</v>
       </c>
       <c r="W9">
-        <v>177.8796296296296</v>
+        <v>175.6785934608267</v>
       </c>
       <c r="X9">
-        <v>159.4845679012346</v>
+        <v>157.0876002467605</v>
       </c>
       <c r="Y9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z9">
-        <v>0.02897547107919962</v>
+        <v>0.02954040164741043</v>
       </c>
       <c r="AA9">
-        <v>453</v>
+        <v>368</v>
       </c>
       <c r="AB9">
-        <v>454</v>
+        <v>392</v>
       </c>
       <c r="AC9">
         <v>54472</v>
       </c>
       <c r="AD9">
-        <v>0.9977973568281938</v>
+        <v>0.9387755102040817</v>
       </c>
       <c r="AE9">
-        <v>0.3836461598056133</v>
+        <v>0.3776064773735581</v>
       </c>
       <c r="AF9">
         <v>0.6177539621785603</v>
       </c>
+      <c r="AG9">
+        <v>29.49881362915039</v>
+      </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G10">
         <v>36600</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I10">
         <v>37.2485728184</v>
@@ -1631,96 +1658,99 @@
         <v>-80.66748366829999</v>
       </c>
       <c r="K10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L10">
-        <v>25.04223198180535</v>
+        <v>24.0497808390732</v>
       </c>
       <c r="M10">
-        <v>63.14359658066034</v>
+        <v>62.21407326236701</v>
       </c>
       <c r="N10">
-        <v>8.312720570935614</v>
+        <v>8.119990607388939</v>
       </c>
       <c r="O10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P10">
-        <v>0.747759932375317</v>
+        <v>0.7199211045364892</v>
       </c>
       <c r="Q10">
-        <v>62.32370557699988</v>
+        <v>57.09934577174681</v>
       </c>
       <c r="R10">
-        <v>95.71103420737388</v>
+        <v>91.42040222922199</v>
       </c>
       <c r="S10">
-        <v>23.58538533209105</v>
+        <v>19.86818512236506</v>
       </c>
       <c r="T10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U10">
-        <v>0.2273316427162581</v>
+        <v>0.2324034939419555</v>
       </c>
       <c r="V10">
-        <v>112.4478764478764</v>
+        <v>98.61520190023751</v>
       </c>
       <c r="W10">
-        <v>133.3526383526383</v>
+        <v>123.4881235154395</v>
       </c>
       <c r="X10">
-        <v>89.80051480051483</v>
+        <v>66.67220902612841</v>
       </c>
       <c r="Y10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Z10">
-        <v>0.02490842490842491</v>
+        <v>0.04767540152155537</v>
       </c>
       <c r="AA10">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB10">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AC10">
-        <v>45085</v>
+        <v>17808</v>
       </c>
       <c r="AD10">
-        <v>0.3577464788732395</v>
+        <v>0.3569405099150141</v>
       </c>
       <c r="AE10">
-        <v>45085</v>
+        <v>0.4003777148253069</v>
       </c>
       <c r="AF10">
-        <v>0</v>
+        <v>0.8890220158753931</v>
+      </c>
+      <c r="AG10">
+        <v>179.0602264404297</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G11">
         <v>36600</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I11">
         <v>37.2504015</v>
@@ -1729,96 +1759,99 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L11">
-        <v>56.73730591691146</v>
+        <v>56.19459603354185</v>
       </c>
       <c r="M11">
-        <v>73.80276961812841</v>
+        <v>73.29189405031292</v>
       </c>
       <c r="N11">
-        <v>24.31542873129109</v>
+        <v>23.76214561426931</v>
       </c>
       <c r="O11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P11">
-        <v>0.4907691331655635</v>
+        <v>0.4761985323661894</v>
       </c>
       <c r="Q11">
-        <v>76.9210566733221</v>
+        <v>76.48937215325529</v>
       </c>
       <c r="R11">
-        <v>93.91952081093535</v>
+        <v>93.34455657765463</v>
       </c>
       <c r="S11">
-        <v>47.44785747197052</v>
+        <v>46.77855675627457</v>
       </c>
       <c r="T11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U11">
-        <v>0.4624103876329647</v>
+        <v>0.473724279400258</v>
       </c>
       <c r="V11">
-        <v>123.2899408284024</v>
+        <v>121.4927782497879</v>
       </c>
       <c r="W11">
-        <v>131.6449704142011</v>
+        <v>130.1444350042481</v>
       </c>
       <c r="X11">
-        <v>109.3076923076923</v>
+        <v>106.4655904842826</v>
       </c>
       <c r="Y11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Z11">
-        <v>0.04682047920147187</v>
+        <v>0.05007718823355256</v>
       </c>
       <c r="AA11">
-        <v>391</v>
+        <v>322</v>
       </c>
       <c r="AB11">
-        <v>394</v>
+        <v>296</v>
       </c>
       <c r="AC11">
         <v>46800</v>
       </c>
       <c r="AD11">
-        <v>0.9923857868020305</v>
+        <v>1.087837837837838</v>
       </c>
       <c r="AE11">
-        <v>0.5007114810574855</v>
+        <v>0.4910189692798388</v>
       </c>
       <c r="AF11">
         <v>0.7538720511602058</v>
       </c>
+      <c r="AG11">
+        <v>87.69241333007812</v>
+      </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G12">
         <v>36600</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I12">
         <v>37.2504015</v>
@@ -1827,96 +1860,99 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L12">
-        <v>50.67990150815636</v>
+        <v>50.45849880857833</v>
       </c>
       <c r="M12">
-        <v>63.9854570637119</v>
+        <v>63.77760127085</v>
       </c>
       <c r="N12">
-        <v>26.6241920590951</v>
+        <v>26.44360603653684</v>
       </c>
       <c r="O12" t="s">
+        <v>108</v>
+      </c>
+      <c r="P12">
+        <v>0.5133537206931702</v>
+      </c>
+      <c r="Q12">
+        <v>69.91886455073768</v>
+      </c>
+      <c r="R12">
+        <v>82.6385784532857</v>
+      </c>
+      <c r="S12">
+        <v>43.39651318730436</v>
+      </c>
+      <c r="T12" t="s">
         <v>107</v>
       </c>
-      <c r="P12">
-        <v>0.5235474006116208</v>
-      </c>
-      <c r="Q12">
-        <v>70.3199668141593</v>
-      </c>
-      <c r="R12">
-        <v>82.94957595870207</v>
-      </c>
-      <c r="S12">
-        <v>43.69321533923303</v>
-      </c>
-      <c r="T12" t="s">
-        <v>106</v>
-      </c>
       <c r="U12">
-        <v>0.4462793068297655</v>
+        <v>0.4560652395514781</v>
       </c>
       <c r="V12">
-        <v>113.9549180327869</v>
+        <v>113.3833333333334</v>
       </c>
       <c r="W12">
-        <v>122.1680327868852</v>
+        <v>121.58</v>
       </c>
       <c r="X12">
-        <v>102.9562841530055</v>
+        <v>102.0833333333333</v>
       </c>
       <c r="Y12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z12">
-        <v>0.03017329255861366</v>
+        <v>0.03058103975535168</v>
       </c>
       <c r="AA12">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="AB12">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="AC12">
         <v>9634</v>
       </c>
       <c r="AD12">
-        <v>1</v>
+        <v>0.6650485436893204</v>
       </c>
       <c r="AE12">
-        <v>0.6326503808773313</v>
+        <v>0.3413648926369499</v>
       </c>
       <c r="AF12">
         <v>0.9440007838910391</v>
       </c>
+      <c r="AG12">
+        <v>179.1753540039062</v>
+      </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G13">
         <v>36660</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I13">
         <v>37.2504015</v>
@@ -1925,194 +1961,200 @@
         <v>-80.66645370000001</v>
       </c>
       <c r="K13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L13">
-        <v>34.66468078412867</v>
+        <v>33.60385088078653</v>
       </c>
       <c r="M13">
-        <v>61.95664484162099</v>
+        <v>60.91964651489427</v>
       </c>
       <c r="N13">
-        <v>15.51691932597968</v>
+        <v>14.9695675074617</v>
       </c>
       <c r="O13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P13">
-        <v>0.6794876582396654</v>
+        <v>0.6380372680085141</v>
       </c>
       <c r="Q13">
-        <v>56.72618453865336</v>
+        <v>54.5344846796657</v>
       </c>
       <c r="R13">
-        <v>81.5252369077307</v>
+        <v>79.82451253481885</v>
       </c>
       <c r="S13">
-        <v>30.53710723192019</v>
+        <v>28.62885793871872</v>
       </c>
       <c r="T13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U13">
-        <v>0.2951193099070167</v>
+        <v>0.3351506777698943</v>
       </c>
       <c r="V13">
-        <v>119.2796657381615</v>
+        <v>117.1255230125523</v>
       </c>
       <c r="W13">
-        <v>132.533704735376</v>
+        <v>130.1910739191073</v>
       </c>
       <c r="X13">
-        <v>119.8880222841225</v>
+        <v>116.4170153417014</v>
       </c>
       <c r="Y13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Z13">
-        <v>0.0253930318533179</v>
+        <v>0.02681205422159155</v>
       </c>
       <c r="AA13">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AB13">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AC13">
-        <v>47422</v>
+        <v>26603</v>
       </c>
       <c r="AD13">
-        <v>0.6908396946564885</v>
+        <v>0.685823754789272</v>
       </c>
       <c r="AE13">
-        <v>47422</v>
+        <v>0.5694257154476765</v>
       </c>
       <c r="AF13">
-        <v>0</v>
+        <v>0.8941433492983782</v>
+      </c>
+      <c r="AG13">
+        <v>177.54052734375</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G14">
         <v>37380</v>
       </c>
       <c r="H14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L14">
-        <v>29.31262158141664</v>
+        <v>28.86380451713413</v>
       </c>
       <c r="M14">
-        <v>62.09486211236984</v>
+        <v>61.72975077881609</v>
       </c>
       <c r="N14">
-        <v>8.833848266392033</v>
+        <v>8.59092679127717</v>
       </c>
       <c r="O14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P14">
-        <v>0.7074820907402494</v>
+        <v>0.6812151764393738</v>
       </c>
       <c r="Q14">
-        <v>46.85687022900764</v>
+        <v>45.62962101836793</v>
       </c>
       <c r="R14">
-        <v>76.28594147582697</v>
+        <v>75.28551499651239</v>
       </c>
       <c r="S14">
-        <v>21.87213740458015</v>
+        <v>20.67937688909557</v>
       </c>
       <c r="T14" t="s">
         <v>106</v>
       </c>
       <c r="U14">
-        <v>0.2598169275669939</v>
+        <v>0.2854205359511807</v>
       </c>
       <c r="V14">
-        <v>109.3086419753087</v>
+        <v>107.7176938369782</v>
       </c>
       <c r="W14">
-        <v>125.7827160493827</v>
+        <v>123.5328031809145</v>
       </c>
       <c r="X14">
-        <v>98.95308641975308</v>
+        <v>96.74353876739542</v>
       </c>
       <c r="Y14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z14">
-        <v>0.0327009816927567</v>
+        <v>0.03336428760944548</v>
       </c>
       <c r="AA14">
-        <v>226</v>
+        <v>163</v>
       </c>
       <c r="AB14">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="AC14">
         <v>15060.5</v>
       </c>
       <c r="AD14">
-        <v>0.9826086956521739</v>
+        <v>0.7511520737327189</v>
       </c>
       <c r="AE14">
-        <v>0.4398510514018691</v>
+        <v>0.4257866613892737</v>
       </c>
       <c r="AF14">
         <v>0.7597871052366058</v>
       </c>
+      <c r="AG14">
+        <v>1.601779818534851</v>
+      </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G15">
         <v>37920</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I15">
         <v>37.2295733</v>
@@ -2121,70 +2163,73 @@
         <v>-80.4139393</v>
       </c>
       <c r="K15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L15">
-        <v>38.77505926979612</v>
+        <v>38.79958611906962</v>
       </c>
       <c r="M15">
-        <v>70.3650545282124</v>
+        <v>70.35775230818136</v>
       </c>
       <c r="N15">
-        <v>12.56076339497393</v>
+        <v>12.62158548233079</v>
       </c>
       <c r="O15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P15">
-        <v>0.6718002392344498</v>
+        <v>0.6709244702665755</v>
       </c>
       <c r="Q15">
-        <v>72.04190536813066</v>
+        <v>71.86120424699567</v>
       </c>
       <c r="R15">
-        <v>102.4348079779333</v>
+        <v>102.3265576976802</v>
       </c>
       <c r="S15">
-        <v>29.77928071292169</v>
+        <v>29.54428611343965</v>
       </c>
       <c r="T15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U15">
-        <v>0.306156015037594</v>
+        <v>0.3058356117566644</v>
       </c>
       <c r="V15">
-        <v>122.1222067039106</v>
+        <v>120.7311926605506</v>
       </c>
       <c r="W15">
-        <v>137.3617318435755</v>
+        <v>136.5348623853213</v>
       </c>
       <c r="X15">
-        <v>100.1494413407822</v>
+        <v>96.94220183486244</v>
       </c>
       <c r="Y15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Z15">
-        <v>0.02204374572795625</v>
+        <v>0.02323991797676008</v>
       </c>
       <c r="AA15">
-        <v>290</v>
+        <v>236</v>
       </c>
       <c r="AB15">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="AC15">
         <v>47232.5</v>
       </c>
       <c r="AD15">
-        <v>0.6373626373626373</v>
+        <v>0.5152838427947598</v>
       </c>
       <c r="AE15">
-        <v>0.4894458145945162</v>
+        <v>0.436981903634076</v>
       </c>
       <c r="AF15">
         <v>0.7729284796714041</v>
+      </c>
+      <c r="AG15">
+        <v>166.9147491455078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>